<commit_message>
Updated data and list.
</commit_message>
<xml_diff>
--- a/list.xlsx
+++ b/list.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="21600" yWindow="8460" windowWidth="51200" windowHeight="28340" tabRatio="500"/>
+    <workbookView xWindow="680" yWindow="460" windowWidth="28120" windowHeight="17540" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="list" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="254" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="249" uniqueCount="94">
   <si>
     <t>ID</t>
   </si>
@@ -203,9 +203,6 @@
     <t>% civilian unemployed</t>
   </si>
   <si>
-    <t>duplicate</t>
-  </si>
-  <si>
     <t>opposite</t>
   </si>
   <si>
@@ -288,9 +285,6 @@
   </si>
   <si>
     <t>% pop affiliated with religious group</t>
-  </si>
-  <si>
-    <t>% pop who drive to work alone</t>
   </si>
   <si>
     <t>pop</t>
@@ -851,10 +845,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:BZ60"/>
+  <dimension ref="A1:BZ59"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="H9" sqref="H9"/>
+    <sheetView tabSelected="1" topLeftCell="A40" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="F44" sqref="F1:F1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -894,7 +888,7 @@
         <v>36</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D2" s="5" t="s">
         <v>5</v>
@@ -909,10 +903,10 @@
         <v>3</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D3" s="6" t="s">
         <v>6</v>
@@ -999,10 +993,10 @@
         <v>4</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D4" s="6" t="s">
         <v>6</v>
@@ -1092,7 +1086,7 @@
         <v>7</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D5" s="6" t="s">
         <v>6</v>
@@ -1179,10 +1173,10 @@
         <v>6</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D6" s="6" t="s">
         <v>6</v>
@@ -1269,10 +1263,10 @@
         <v>7</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D7" s="5" t="s">
         <v>8</v>
@@ -1287,10 +1281,10 @@
         <v>8</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D8" s="5" t="s">
         <v>8</v>
@@ -1305,10 +1299,10 @@
         <v>9</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D9" s="5" t="s">
         <v>8</v>
@@ -1326,7 +1320,7 @@
         <v>37</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D10" s="5" t="s">
         <v>8</v>
@@ -1341,10 +1335,10 @@
         <v>11</v>
       </c>
       <c r="B11" s="7" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C11" s="7" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D11" s="7" t="s">
         <v>9</v>
@@ -1434,7 +1428,7 @@
         <v>38</v>
       </c>
       <c r="C12" s="7" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D12" s="7" t="s">
         <v>9</v>
@@ -1524,7 +1518,7 @@
         <v>43</v>
       </c>
       <c r="C13" s="7" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D13" s="7" t="s">
         <v>9</v>
@@ -1614,7 +1608,7 @@
         <v>44</v>
       </c>
       <c r="C14" s="7" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D14" s="7" t="s">
         <v>9</v>
@@ -1704,7 +1698,7 @@
         <v>42</v>
       </c>
       <c r="C15" s="5" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D15" s="5" t="s">
         <v>10</v>
@@ -1722,7 +1716,7 @@
         <v>45</v>
       </c>
       <c r="C16" s="5" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D16" s="5" t="s">
         <v>10</v>
@@ -1737,19 +1731,19 @@
         <v>17</v>
       </c>
       <c r="B17" s="8" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C17" s="8" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D17" s="8" t="s">
         <v>10</v>
       </c>
       <c r="E17" s="8" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F17" s="8" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="18" spans="1:78" ht="32" x14ac:dyDescent="0.2">
@@ -1757,10 +1751,10 @@
         <v>18</v>
       </c>
       <c r="B18" s="5" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="C18" s="5" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D18" s="5" t="s">
         <v>10</v>
@@ -1778,16 +1772,16 @@
         <v>46</v>
       </c>
       <c r="C19" s="9" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D19" s="9" t="s">
         <v>11</v>
       </c>
       <c r="E19" s="9" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F19" s="9" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="G19" s="25"/>
       <c r="H19" s="25"/>
@@ -1867,10 +1861,10 @@
         <v>20</v>
       </c>
       <c r="B20" s="10" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="C20" s="10" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D20" s="10" t="s">
         <v>11</v>
@@ -1957,10 +1951,10 @@
         <v>21</v>
       </c>
       <c r="B21" s="10" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C21" s="10" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D21" s="10" t="s">
         <v>11</v>
@@ -2050,16 +2044,16 @@
         <v>47</v>
       </c>
       <c r="C22" s="9" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D22" s="9" t="s">
         <v>11</v>
       </c>
       <c r="E22" s="9" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="F22" s="9" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="G22" s="25"/>
       <c r="H22" s="25"/>
@@ -2139,10 +2133,10 @@
         <v>23</v>
       </c>
       <c r="B23" s="5" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C23" s="5" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D23" s="5" t="s">
         <v>12</v>
@@ -2157,10 +2151,10 @@
         <v>24</v>
       </c>
       <c r="B24" s="5" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C24" s="5" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D24" s="5" t="s">
         <v>12</v>
@@ -2178,7 +2172,7 @@
         <v>48</v>
       </c>
       <c r="C25" s="5" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D25" s="5" t="s">
         <v>12</v>
@@ -2196,7 +2190,7 @@
         <v>49</v>
       </c>
       <c r="C26" s="5" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D26" s="5" t="s">
         <v>12</v>
@@ -2214,7 +2208,7 @@
         <v>50</v>
       </c>
       <c r="C27" s="5" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D27" s="5" t="s">
         <v>12</v>
@@ -2232,7 +2226,7 @@
         <v>51</v>
       </c>
       <c r="C28" s="11" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D28" s="11" t="s">
         <v>15</v>
@@ -2322,7 +2316,7 @@
         <v>52</v>
       </c>
       <c r="C29" s="11" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D29" s="11" t="s">
         <v>15</v>
@@ -2409,10 +2403,10 @@
         <v>32</v>
       </c>
       <c r="B30" s="12" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C30" s="12" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D30" s="12" t="s">
         <v>15</v>
@@ -2421,7 +2415,7 @@
         <v>33</v>
       </c>
       <c r="F30" s="12" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="G30" s="25"/>
       <c r="H30" s="25"/>
@@ -2504,7 +2498,7 @@
         <v>53</v>
       </c>
       <c r="C31" s="5" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D31" s="5" t="s">
         <v>16</v>
@@ -2519,10 +2513,10 @@
         <v>42</v>
       </c>
       <c r="B32" s="13" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C32" s="13" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D32" s="13" t="s">
         <v>17</v>
@@ -2612,7 +2606,7 @@
         <v>54</v>
       </c>
       <c r="C33" s="14" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D33" s="14" t="s">
         <v>17</v>
@@ -2702,7 +2696,7 @@
         <v>35</v>
       </c>
       <c r="C34" s="13" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D34" s="13" t="s">
         <v>17</v>
@@ -2792,7 +2786,7 @@
         <v>39</v>
       </c>
       <c r="C35" s="5" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D35" s="5" t="s">
         <v>18</v>
@@ -2810,7 +2804,7 @@
         <v>19</v>
       </c>
       <c r="C36" s="5" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D36" s="5" t="s">
         <v>18</v>
@@ -2828,7 +2822,7 @@
         <v>55</v>
       </c>
       <c r="C37" s="5" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D37" s="5" t="s">
         <v>18</v>
@@ -2846,7 +2840,7 @@
         <v>21</v>
       </c>
       <c r="C38" s="5" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D38" s="5" t="s">
         <v>18</v>
@@ -2864,7 +2858,7 @@
         <v>23</v>
       </c>
       <c r="C39" s="5" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D39" s="5" t="s">
         <v>18</v>
@@ -2882,7 +2876,7 @@
         <v>56</v>
       </c>
       <c r="C40" s="5" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D40" s="5" t="s">
         <v>18</v>
@@ -2891,7 +2885,7 @@
         <v>34</v>
       </c>
       <c r="F40" s="5" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
     </row>
     <row r="41" spans="1:78" ht="32" x14ac:dyDescent="0.2">
@@ -2902,7 +2896,7 @@
         <v>57</v>
       </c>
       <c r="C41" s="5" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D41" s="5" t="s">
         <v>18</v>
@@ -2911,7 +2905,7 @@
         <v>34</v>
       </c>
       <c r="F41" s="5" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
     </row>
     <row r="42" spans="1:78" ht="32" x14ac:dyDescent="0.2">
@@ -2919,10 +2913,10 @@
         <v>54</v>
       </c>
       <c r="B42" s="5" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C42" s="5" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D42" s="5" t="s">
         <v>18</v>
@@ -2937,7 +2931,7 @@
         <v>55</v>
       </c>
       <c r="B43" s="15" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C43" s="15" t="s">
         <v>24</v>
@@ -2946,10 +2940,10 @@
         <v>25</v>
       </c>
       <c r="E43" s="15" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F43" s="15" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="G43" s="25"/>
       <c r="H43" s="25"/>
@@ -3029,7 +3023,7 @@
         <v>56</v>
       </c>
       <c r="B44" s="16" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C44" s="16" t="s">
         <v>24</v>
@@ -3119,7 +3113,7 @@
         <v>57</v>
       </c>
       <c r="B45" s="16" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C45" s="16" t="s">
         <v>24</v>
@@ -3209,7 +3203,7 @@
         <v>60</v>
       </c>
       <c r="B46" s="16" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C46" s="16" t="s">
         <v>24</v>
@@ -3317,7 +3311,7 @@
         <v>64</v>
       </c>
       <c r="B48" s="17" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C48" s="17" t="s">
         <v>24</v>
@@ -3407,7 +3401,7 @@
         <v>65</v>
       </c>
       <c r="B49" s="18" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C49" s="18" t="s">
         <v>24</v>
@@ -3497,7 +3491,7 @@
         <v>66</v>
       </c>
       <c r="B50" s="18" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C50" s="18" t="s">
         <v>24</v>
@@ -3677,7 +3671,7 @@
         <v>69</v>
       </c>
       <c r="B52" s="18" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C52" s="18" t="s">
         <v>24</v>
@@ -3767,10 +3761,10 @@
         <v>73</v>
       </c>
       <c r="B53" s="5" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C53" s="5" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D53" s="5" t="s">
         <v>29</v>
@@ -3785,10 +3779,10 @@
         <v>74</v>
       </c>
       <c r="B54" s="5" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C54" s="5" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D54" s="5" t="s">
         <v>29</v>
@@ -3806,68 +3800,66 @@
         <v>40</v>
       </c>
       <c r="C55" s="8" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D55" s="8" t="s">
         <v>29</v>
       </c>
       <c r="E55" s="8" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="F55" s="8" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="56" spans="1:78" s="25" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A56" s="24">
-        <v>76</v>
-      </c>
-      <c r="B56" s="8" t="s">
-        <v>88</v>
-      </c>
-      <c r="C56" s="8" t="s">
-        <v>63</v>
-      </c>
-      <c r="D56" s="8" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="56" spans="1:78" x14ac:dyDescent="0.2">
+      <c r="A56" s="19">
+        <v>77</v>
+      </c>
+      <c r="B56" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="C56" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="D56" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="E56" s="8" t="s">
+      <c r="E56" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="F56" s="8" t="s">
-        <v>59</v>
-      </c>
+      <c r="F56" s="5"/>
     </row>
     <row r="57" spans="1:78" x14ac:dyDescent="0.2">
       <c r="A57" s="19">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="B57" s="5" t="s">
-        <v>41</v>
+        <v>64</v>
       </c>
       <c r="C57" s="5" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D57" s="5" t="s">
         <v>29</v>
       </c>
       <c r="E57" s="5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F57" s="5"/>
     </row>
     <row r="58" spans="1:78" x14ac:dyDescent="0.2">
       <c r="A58" s="19">
-        <v>78</v>
+        <v>902</v>
       </c>
       <c r="B58" s="5" t="s">
-        <v>65</v>
+        <v>93</v>
       </c>
       <c r="C58" s="5" t="s">
-        <v>63</v>
+        <v>30</v>
       </c>
       <c r="D58" s="5" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="E58" s="5" t="s">
         <v>33</v>
@@ -3876,39 +3868,21 @@
     </row>
     <row r="59" spans="1:78" x14ac:dyDescent="0.2">
       <c r="A59" s="19">
-        <v>902</v>
+        <v>901</v>
       </c>
       <c r="B59" s="5" t="s">
-        <v>95</v>
+        <v>87</v>
       </c>
       <c r="C59" s="5" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="D59" s="5" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="E59" s="5" t="s">
         <v>33</v>
       </c>
       <c r="F59" s="5"/>
-    </row>
-    <row r="60" spans="1:78" x14ac:dyDescent="0.2">
-      <c r="A60" s="19">
-        <v>901</v>
-      </c>
-      <c r="B60" s="5" t="s">
-        <v>89</v>
-      </c>
-      <c r="C60" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="D60" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="E60" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="F60" s="5"/>
     </row>
   </sheetData>
   <phoneticPr fontId="4" type="noConversion"/>

</xml_diff>